<commit_message>
updated Marilao Long Lat
</commit_message>
<xml_diff>
--- a/DataSets/Marilao shelter data.xlsx
+++ b/DataSets/Marilao shelter data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL\BRYAN\bulsu\Thesis 1\ShelterAlloc_Thesis\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5946BD-5082-4500-AAFB-200E064768BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C989421F-3FA8-467C-9592-FD51CD818DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:W999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -538,10 +538,10 @@
         <v>20</v>
       </c>
       <c r="B2">
+        <v>14.7718799806491</v>
+      </c>
+      <c r="C2">
         <v>120.94091440622999</v>
-      </c>
-      <c r="C2">
-        <v>14.7718799806491</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -576,10 +576,10 @@
         <v>22</v>
       </c>
       <c r="B3">
+        <v>14.775252992136499</v>
+      </c>
+      <c r="C3">
         <v>120.94426552157699</v>
-      </c>
-      <c r="C3">
-        <v>14.775252992136499</v>
       </c>
       <c r="D3">
         <v>240</v>
@@ -614,10 +614,10 @@
         <v>23</v>
       </c>
       <c r="B4">
+        <v>14.7712372258247</v>
+      </c>
+      <c r="C4">
         <v>120.943458029502</v>
-      </c>
-      <c r="C4">
-        <v>14.7712372258247</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -652,10 +652,10 @@
         <v>24</v>
       </c>
       <c r="B5">
+        <v>14.769618908499501</v>
+      </c>
+      <c r="C5">
         <v>120.93696006008599</v>
-      </c>
-      <c r="C5">
-        <v>14.769618908499501</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -690,10 +690,10 @@
         <v>25</v>
       </c>
       <c r="B6">
+        <v>14.764714339619699</v>
+      </c>
+      <c r="C6">
         <v>120.942286137427</v>
-      </c>
-      <c r="C6">
-        <v>14.764714339619699</v>
       </c>
       <c r="D6">
         <v>720</v>
@@ -728,10 +728,10 @@
         <v>26</v>
       </c>
       <c r="B7">
+        <v>14.7535649557989</v>
+      </c>
+      <c r="C7">
         <v>120.959816737558</v>
-      </c>
-      <c r="C7">
-        <v>14.7535649557989</v>
       </c>
       <c r="D7">
         <v>150</v>
@@ -766,10 +766,10 @@
         <v>27</v>
       </c>
       <c r="B8">
+        <v>14.7713627238379</v>
+      </c>
+      <c r="C8">
         <v>120.97521021538699</v>
-      </c>
-      <c r="C8">
-        <v>14.7713627238379</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -804,10 +804,10 @@
         <v>28</v>
       </c>
       <c r="B9">
+        <v>14.762777944714299</v>
+      </c>
+      <c r="C9">
         <v>120.965390844846</v>
-      </c>
-      <c r="C9">
-        <v>14.762777944714299</v>
       </c>
       <c r="D9">
         <v>448</v>
@@ -842,10 +842,10 @@
         <v>41</v>
       </c>
       <c r="B10">
+        <v>14.783955314095699</v>
+      </c>
+      <c r="C10">
         <v>121.02706273692399</v>
-      </c>
-      <c r="C10">
-        <v>14.783955314095699</v>
       </c>
       <c r="D10">
         <v>300</v>
@@ -880,10 +880,10 @@
         <v>29</v>
       </c>
       <c r="B11">
+        <v>14.7549081782114</v>
+      </c>
+      <c r="C11">
         <v>120.94919107604299</v>
-      </c>
-      <c r="C11">
-        <v>14.7549081782114</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -918,10 +918,10 @@
         <v>39</v>
       </c>
       <c r="B12">
+        <v>14.7523618894178</v>
+      </c>
+      <c r="C12">
         <v>120.95078829138799</v>
-      </c>
-      <c r="C12">
-        <v>14.7523618894178</v>
       </c>
       <c r="D12">
         <v>100</v>
@@ -956,10 +956,10 @@
         <v>30</v>
       </c>
       <c r="B13">
+        <v>14.7788884149633</v>
+      </c>
+      <c r="C13">
         <v>120.960345299663</v>
-      </c>
-      <c r="C13">
-        <v>14.7788884149633</v>
       </c>
       <c r="D13">
         <v>75</v>
@@ -994,10 +994,10 @@
         <v>31</v>
       </c>
       <c r="B14">
+        <v>14.757300686139599</v>
+      </c>
+      <c r="C14">
         <v>120.948177254006</v>
-      </c>
-      <c r="C14">
-        <v>14.757300686139599</v>
       </c>
       <c r="D14">
         <v>75</v>
@@ -1032,10 +1032,10 @@
         <v>32</v>
       </c>
       <c r="B15">
+        <v>14.759696361212599</v>
+      </c>
+      <c r="C15">
         <v>120.94380312195401</v>
-      </c>
-      <c r="C15">
-        <v>14.759696361212599</v>
       </c>
       <c r="D15">
         <v>1800</v>
@@ -1070,10 +1070,10 @@
         <v>33</v>
       </c>
       <c r="B16">
+        <v>14.783636298137299</v>
+      </c>
+      <c r="C16">
         <v>120.984338290888</v>
-      </c>
-      <c r="C16">
-        <v>14.783636298137299</v>
       </c>
       <c r="D16">
         <v>120</v>
@@ -1108,10 +1108,10 @@
         <v>34</v>
       </c>
       <c r="B17">
+        <v>14.765465938427001</v>
+      </c>
+      <c r="C17">
         <v>120.95619816761101</v>
-      </c>
-      <c r="C17">
-        <v>14.765465938427001</v>
       </c>
       <c r="D17">
         <v>500</v>
@@ -1146,10 +1146,10 @@
         <v>35</v>
       </c>
       <c r="B18">
+        <v>14.764617728072199</v>
+      </c>
+      <c r="C18">
         <v>120.954403339867</v>
-      </c>
-      <c r="C18">
-        <v>14.764617728072199</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1184,10 +1184,10 @@
         <v>36</v>
       </c>
       <c r="B19">
+        <v>14.778956209200601</v>
+      </c>
+      <c r="C19">
         <v>120.973228584392</v>
-      </c>
-      <c r="C19">
-        <v>14.778956209200601</v>
       </c>
       <c r="D19">
         <v>200</v>
@@ -1222,10 +1222,10 @@
         <v>37</v>
       </c>
       <c r="B20">
+        <v>14.7865722729873</v>
+      </c>
+      <c r="C20">
         <v>120.968978114161</v>
-      </c>
-      <c r="C20">
-        <v>14.7865722729873</v>
       </c>
       <c r="D20">
         <v>1615</v>
@@ -1260,10 +1260,10 @@
         <v>40</v>
       </c>
       <c r="B21">
+        <v>14.7656033896092</v>
+      </c>
+      <c r="C21">
         <v>120.948513036352</v>
-      </c>
-      <c r="C21">
-        <v>14.7656033896092</v>
       </c>
       <c r="D21">
         <v>272</v>
@@ -1298,10 +1298,10 @@
         <v>38</v>
       </c>
       <c r="B22">
+        <v>14.7652274561484</v>
+      </c>
+      <c r="C22">
         <v>120.948821314155</v>
-      </c>
-      <c r="C22">
-        <v>14.7652274561484</v>
       </c>
       <c r="D22">
         <v>798</v>

</xml_diff>